<commit_message>
Fix reference to column name bug
</commit_message>
<xml_diff>
--- a/data/excel_files_raw/test_excel_1_raw.xlsx
+++ b/data/excel_files_raw/test_excel_1_raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrislittle/GitHub/speedsheet/mvp/data/excel_files_clean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrislittle/GitHub/speedsheet/excel-2-python/data/excel_files_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3443902C-F142-ED46-9B17-0EB5C24EC9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11989BB-33AF-6E4E-88AA-33170DEA7A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>col_1</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>col_4</t>
-  </si>
-  <si>
-    <t>col_5</t>
   </si>
   <si>
     <t>horizontal_col_1</t>
@@ -475,7 +472,7 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <f>B3</f>
@@ -488,7 +485,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <f>B4</f>
@@ -562,7 +559,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -573,7 +570,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -584,23 +581,23 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <f>B2+B3</f>
         <v>5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:D4" si="0">C2+C3</f>
+        <f t="shared" ref="C4" si="0">C2+C3</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -615,7 +612,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" ref="A12:B13" si="1">B3</f>
+        <f t="shared" ref="A12:B12" si="1">B3</f>
         <v>4</v>
       </c>
       <c r="B12">
@@ -631,15 +628,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -652,11 +649,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(Sheet1!$B$2:$B$6)</f>
         <v>4</v>
@@ -669,16 +663,12 @@
         <f>SUM(Sheet1!$D$2:$D$6)</f>
         <v>10</v>
       </c>
-      <c r="D2" t="str">
-        <f>INDEX(Sheet1!E:E,MATCH(Sheet3!D1,Sheet1!E:E,0))</f>
-        <v>col_4</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <f>Sheet3!A2*Sheet3!B2</f>
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>SUM(Sheet1!$B$2:$B$6)</f>
         <v>4</v>
@@ -691,11 +681,7 @@
         <f>SUM(Sheet1!$D$2:$D$6)</f>
         <v>10</v>
       </c>
-      <c r="D3" t="str">
-        <f>INDEX(Sheet1!E:E,MATCH(Sheet3!D2,Sheet1!E:E,0))</f>
-        <v>col_4</v>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <f>Sheet3!A3*Sheet3!B3</f>
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Fix Excel Validation issue
</commit_message>
<xml_diff>
--- a/data/excel_files_raw/test_excel_1_raw.xlsx
+++ b/data/excel_files_raw/test_excel_1_raw.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrislittle/GitHub/speedsheet/excel-2-python/data/excel_files_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC3110F-4B7A-DB49-ACA1-48DCA5CF0558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5717C158-ACE4-9048-B332-14004FF6F708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>col_1</t>
   </si>
@@ -415,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
@@ -625,69 +624,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <f>SUM(Sheet1!$B$2:$B$6)</f>
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <f>SUM(Sheet1!$C$2:$C$6)</f>
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <f>SUM(Sheet1!$D$2:$D$6)</f>
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <f>Sheet3!A2*Sheet3!B2</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f>SUM(Sheet1!$B$2:$B$6)</f>
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <f>SUM(Sheet1!$C$2:$C$6)</f>
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <f>SUM(Sheet1!$D$2:$D$6)</f>
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <f>Sheet3!A3*Sheet3!B3</f>
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>